<commit_message>
fix export excel phieu muon
</commit_message>
<xml_diff>
--- a/QuanLyThuVienHUFI/Form_QuanLyThuVien/bin/Debug/DSPMTHCT.xlsx
+++ b/QuanLyThuVienHUFI/Form_QuanLyThuVien/bin/Debug/DSPMTHCT.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevPrograms\DATN_25_12_2020\DATN_QuanLyThuVienHUFI_LamDat(25_12)\QuanLyThuVienHUFI\Form_QuanLyThuVien\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevPrograms\GitHub\DATN\HUFILibrary\QuanLyThuVienHUFI\Form_QuanLyThuVien\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="phieumuon">Sheet1!$B$13:$F$13</definedName>
+    <definedName name="phieumuon">Sheet1!$B$13:$G$13</definedName>
   </definedNames>
   <calcPr calcId="162913" iterateDelta="0"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>TRUNG TÂM THÔNG TIN THƯ VIỆN</t>
   </si>
@@ -71,16 +71,22 @@
     <t>{thoihanmuon}</t>
   </si>
   <si>
-    <t>Phí cọc</t>
-  </si>
-  <si>
-    <t>{phicoc}</t>
-  </si>
-  <si>
     <t>Họ và tên người in:</t>
   </si>
   <si>
     <t>Mã số thẻ người in:</t>
+  </si>
+  <si>
+    <t>Số lượng tài liệu trễ</t>
+  </si>
+  <si>
+    <t>{soluongtailieutre}</t>
+  </si>
+  <si>
+    <t>Số ngày trễ</t>
+  </si>
+  <si>
+    <t>{songaytre}</t>
   </si>
 </sst>
 </file>
@@ -142,7 +148,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -178,11 +184,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -200,6 +232,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -217,9 +260,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -504,7 +544,7 @@
   <dimension ref="B1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -518,58 +558,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
     </row>
     <row r="2" spans="2:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
     </row>
     <row r="7" spans="2:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="15"/>
+      <c r="D7" s="13"/>
     </row>
     <row r="8" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="2:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="15"/>
+      <c r="D9" s="13"/>
     </row>
     <row r="11" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="12" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -585,8 +625,11 @@
       <c r="E12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>14</v>
+      <c r="F12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -603,7 +646,10 @@
         <v>13</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -612,6 +658,7 @@
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
+      <c r="G14" s="10"/>
     </row>
     <row r="15" spans="2:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="4"/>
@@ -619,6 +666,7 @@
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
+      <c r="G15" s="9"/>
     </row>
     <row r="17" spans="4:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D17" s="8"/>

</xml_diff>